<commit_message>
managed case nb lines client ID > invoice details and + btn to compute taxe d'ameublement
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5DA209-F2E2-4596-844D-1CFE4BCB3C31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DC843-76CB-4BAC-BE21-FF7AAC012462}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -198,6 +199,15 @@
   </si>
   <si>
     <t>Validation de facture: sauvegarde des infos du client en gérant les cas où le formulaire serait modifié, enrichi ou appauvri</t>
+  </si>
+  <si>
+    <t>Gestion du cas ou l'on voudrait ajouter des infos à l'identification du client ou aux détails de la facture alors que les deux blocs ne sont pas de la même taille</t>
+  </si>
+  <si>
+    <t>Affectation d'un bouton dédié pour mettre à jour le calcul de la taxe d'ameublement si besoin</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -279,12 +289,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="120"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="120"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="120"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="120"/>
     </xf>
   </cellXfs>
@@ -604,8 +614,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="C1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E38" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59:L61"/>
+    <sheetView tabSelected="1" topLeftCell="H56" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +652,7 @@
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="4">
         <v>44292</v>
       </c>
       <c r="L3">
@@ -660,7 +670,7 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="4"/>
       <c r="K4" t="s">
         <v>25</v>
       </c>
@@ -675,7 +685,7 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="4"/>
       <c r="K5" t="s">
         <v>26</v>
       </c>
@@ -690,7 +700,7 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="4"/>
       <c r="K6" t="s">
         <v>46</v>
       </c>
@@ -705,7 +715,7 @@
       <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="4"/>
       <c r="K7" t="s">
         <v>27</v>
       </c>
@@ -720,7 +730,7 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="4"/>
       <c r="K8" t="s">
         <v>28</v>
       </c>
@@ -738,7 +748,7 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="4"/>
       <c r="K9" t="s">
         <v>48</v>
       </c>
@@ -753,7 +763,7 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="4"/>
       <c r="K10" t="s">
         <v>47</v>
       </c>
@@ -776,7 +786,7 @@
       <c r="E12" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="5">
         <v>44293</v>
       </c>
       <c r="L12">
@@ -785,7 +795,7 @@
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J13" s="4"/>
+      <c r="J13" s="5"/>
       <c r="K13" t="s">
         <v>29</v>
       </c>
@@ -803,7 +813,7 @@
       <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="4"/>
+      <c r="J14" s="5"/>
       <c r="K14" t="s">
         <v>30</v>
       </c>
@@ -812,7 +822,7 @@
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J15" s="4"/>
+      <c r="J15" s="5"/>
       <c r="K15" t="s">
         <v>31</v>
       </c>
@@ -830,7 +840,7 @@
       <c r="E16" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="4"/>
+      <c r="J16" s="5"/>
       <c r="K16" t="s">
         <v>32</v>
       </c>
@@ -848,7 +858,7 @@
       <c r="E18" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="5">
         <v>44294</v>
       </c>
       <c r="L18">
@@ -863,7 +873,7 @@
       <c r="E19" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="4"/>
+      <c r="J19" s="5"/>
       <c r="K19" t="s">
         <v>33</v>
       </c>
@@ -881,7 +891,7 @@
       <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="4"/>
+      <c r="J20" s="5"/>
       <c r="K20" t="s">
         <v>37</v>
       </c>
@@ -896,7 +906,7 @@
       <c r="E21" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="4"/>
+      <c r="J21" s="5"/>
       <c r="K21" t="s">
         <v>34</v>
       </c>
@@ -905,7 +915,7 @@
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J22" s="4"/>
+      <c r="J22" s="5"/>
       <c r="K22" t="s">
         <v>35</v>
       </c>
@@ -928,7 +938,7 @@
       <c r="E24" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="3">
         <v>44295</v>
       </c>
       <c r="L24">
@@ -937,7 +947,7 @@
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J25" s="5"/>
+      <c r="J25" s="3"/>
       <c r="K25" t="s">
         <v>39</v>
       </c>
@@ -955,7 +965,7 @@
       <c r="E26" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="5"/>
+      <c r="J26" s="3"/>
       <c r="K26" t="s">
         <v>36</v>
       </c>
@@ -970,7 +980,7 @@
       <c r="E27" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="J27" s="3"/>
       <c r="K27" t="s">
         <v>38</v>
       </c>
@@ -979,13 +989,13 @@
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J28" s="5"/>
+      <c r="J28" s="3"/>
       <c r="K28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J31" s="5">
+      <c r="J31" s="3">
         <v>44296</v>
       </c>
       <c r="L31">
@@ -994,7 +1004,7 @@
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J32" s="5"/>
+      <c r="J32" s="3"/>
       <c r="K32" t="s">
         <v>39</v>
       </c>
@@ -1003,7 +1013,7 @@
       </c>
     </row>
     <row r="33" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J33" s="5"/>
+      <c r="J33" s="3"/>
       <c r="K33" t="s">
         <v>40</v>
       </c>
@@ -1012,7 +1022,7 @@
       </c>
     </row>
     <row r="34" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J34" s="5"/>
+      <c r="J34" s="3"/>
       <c r="K34" t="s">
         <v>41</v>
       </c>
@@ -1021,7 +1031,7 @@
       </c>
     </row>
     <row r="35" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J35" s="5"/>
+      <c r="J35" s="3"/>
       <c r="K35" t="s">
         <v>42</v>
       </c>
@@ -1030,7 +1040,7 @@
       </c>
     </row>
     <row r="36" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J36" s="5"/>
+      <c r="J36" s="3"/>
       <c r="K36" t="s">
         <v>43</v>
       </c>
@@ -1039,7 +1049,7 @@
       </c>
     </row>
     <row r="37" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J37" s="5"/>
+      <c r="J37" s="3"/>
       <c r="K37" t="s">
         <v>44</v>
       </c>
@@ -1048,7 +1058,7 @@
       </c>
     </row>
     <row r="38" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J38" s="5"/>
+      <c r="J38" s="3"/>
       <c r="K38" t="s">
         <v>45</v>
       </c>
@@ -1057,12 +1067,12 @@
       </c>
     </row>
     <row r="40" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J40" s="5">
+      <c r="J40" s="3">
         <v>44297</v>
       </c>
     </row>
     <row r="41" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J41" s="5"/>
+      <c r="J41" s="3"/>
       <c r="K41" t="s">
         <v>50</v>
       </c>
@@ -1071,13 +1081,13 @@
       </c>
     </row>
     <row r="42" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J42" s="5"/>
+      <c r="J42" s="3"/>
     </row>
     <row r="43" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J43" s="5"/>
+      <c r="J43" s="3"/>
     </row>
     <row r="44" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J44" s="5"/>
+      <c r="J44" s="3"/>
     </row>
     <row r="47" spans="10:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="K47" s="2" t="s">
@@ -1085,16 +1095,16 @@
       </c>
       <c r="L47">
         <f>L48+L57+L63+L69+L76+L86</f>
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J48" s="3">
+      <c r="J48" s="4">
         <v>44298</v>
       </c>
     </row>
     <row r="49" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J49" s="3"/>
+      <c r="J49" s="4"/>
       <c r="K49" t="s">
         <v>54</v>
       </c>
@@ -1103,29 +1113,29 @@
       </c>
     </row>
     <row r="50" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J50" s="3"/>
+      <c r="J50" s="4"/>
       <c r="K50" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="51" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J51" s="3"/>
+      <c r="J51" s="4"/>
     </row>
     <row r="52" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J52" s="3"/>
+      <c r="J52" s="4"/>
     </row>
     <row r="53" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J53" s="3"/>
+      <c r="J53" s="4"/>
     </row>
     <row r="54" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J54" s="3"/>
+      <c r="J54" s="4"/>
     </row>
     <row r="55" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J55" s="3"/>
+      <c r="J55" s="4"/>
     </row>
     <row r="57" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J57" s="4">
-        <v>44293</v>
+      <c r="J57" s="5">
+        <v>44299</v>
       </c>
       <c r="L57">
         <f>SUM(L58:L61)</f>
@@ -1133,7 +1143,7 @@
       </c>
     </row>
     <row r="58" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J58" s="4"/>
+      <c r="J58" s="5"/>
       <c r="K58" t="s">
         <v>54</v>
       </c>
@@ -1142,180 +1152,109 @@
       </c>
     </row>
     <row r="59" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J59" s="4"/>
+      <c r="J59" s="5"/>
     </row>
     <row r="60" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J60" s="4"/>
+      <c r="J60" s="5"/>
     </row>
     <row r="61" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J61" s="4"/>
+      <c r="J61" s="5"/>
     </row>
     <row r="63" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J63" s="4">
-        <v>44294</v>
+      <c r="J63" s="5">
+        <f>J57+1</f>
+        <v>44300</v>
       </c>
       <c r="L63">
         <f>SUM(L64:L67)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J64" s="4"/>
-      <c r="K64" t="s">
-        <v>33</v>
-      </c>
-      <c r="L64">
-        <v>1</v>
-      </c>
+      <c r="J64" s="5"/>
     </row>
     <row r="65" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J65" s="4"/>
-      <c r="K65" t="s">
-        <v>37</v>
-      </c>
-      <c r="L65">
-        <v>3</v>
-      </c>
+      <c r="J65" s="5"/>
     </row>
     <row r="66" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J66" s="4"/>
-      <c r="K66" t="s">
-        <v>34</v>
-      </c>
-      <c r="L66">
-        <v>2</v>
-      </c>
+      <c r="J66" s="5"/>
     </row>
     <row r="67" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J67" s="4"/>
-      <c r="K67" t="s">
-        <v>35</v>
-      </c>
-      <c r="L67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J67" s="5"/>
+    </row>
+    <row r="69" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J69" s="5">
-        <v>44295</v>
+        <f>J63+1</f>
+        <v>44301</v>
       </c>
       <c r="L69">
         <f>SUM(L70:L72)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J70" s="5"/>
-      <c r="K70" t="s">
-        <v>39</v>
-      </c>
-      <c r="L70">
-        <v>2</v>
-      </c>
     </row>
     <row r="71" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J71" s="5"/>
-      <c r="K71" t="s">
-        <v>36</v>
-      </c>
-      <c r="L71">
-        <v>1</v>
-      </c>
     </row>
     <row r="72" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J72" s="5"/>
-      <c r="K72" t="s">
-        <v>38</v>
-      </c>
-      <c r="L72">
-        <v>2</v>
-      </c>
     </row>
     <row r="73" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J73" s="5"/>
-      <c r="K73" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="76" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J76" s="5">
-        <v>44296</v>
+      <c r="J76" s="3">
+        <f>J69+1</f>
+        <v>44302</v>
       </c>
       <c r="L76">
         <f>SUM(L77:L83)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J77" s="5"/>
+      <c r="J77" s="3"/>
       <c r="K77" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="L77">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J78" s="5"/>
+      <c r="J78" s="3"/>
       <c r="K78" t="s">
-        <v>40</v>
-      </c>
-      <c r="L78">
-        <v>2</v>
+        <v>56</v>
+      </c>
+      <c r="L78" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="79" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J79" s="5"/>
-      <c r="K79" t="s">
-        <v>41</v>
-      </c>
-      <c r="L79">
-        <v>0.5</v>
-      </c>
+      <c r="J79" s="3"/>
     </row>
     <row r="80" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J80" s="5"/>
-      <c r="K80" t="s">
-        <v>42</v>
-      </c>
-      <c r="L80">
-        <v>1</v>
-      </c>
+      <c r="J80" s="3"/>
     </row>
     <row r="81" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J81" s="5"/>
-      <c r="K81" t="s">
-        <v>43</v>
-      </c>
-      <c r="L81">
-        <v>1</v>
-      </c>
+      <c r="J81" s="3"/>
     </row>
     <row r="82" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J82" s="5"/>
-      <c r="K82" t="s">
-        <v>44</v>
-      </c>
-      <c r="L82">
-        <v>1</v>
-      </c>
+      <c r="J82" s="3"/>
     </row>
     <row r="83" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J83" s="5"/>
-      <c r="K83" t="s">
-        <v>45</v>
-      </c>
-      <c r="L83">
-        <v>0.5</v>
-      </c>
+      <c r="J83" s="3"/>
     </row>
     <row r="85" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J85" s="5">
-        <v>44297</v>
+      <c r="J85" s="3">
+        <f>J76+1</f>
+        <v>44303</v>
       </c>
     </row>
     <row r="86" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J86" s="5"/>
+      <c r="J86" s="3"/>
       <c r="K86" t="s">
         <v>50</v>
       </c>
@@ -1324,16 +1263,21 @@
       </c>
     </row>
     <row r="87" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J87" s="5"/>
+      <c r="J87" s="3"/>
     </row>
     <row r="88" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J88" s="5"/>
+      <c r="J88" s="3"/>
     </row>
     <row r="89" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J89" s="5"/>
+      <c r="J89" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="J3:J10"/>
+    <mergeCell ref="J12:J16"/>
+    <mergeCell ref="J18:J22"/>
+    <mergeCell ref="J24:J28"/>
+    <mergeCell ref="J31:J38"/>
     <mergeCell ref="J76:J83"/>
     <mergeCell ref="J85:J89"/>
     <mergeCell ref="J40:J44"/>
@@ -1341,11 +1285,6 @@
     <mergeCell ref="J57:J61"/>
     <mergeCell ref="J63:J67"/>
     <mergeCell ref="J69:J73"/>
-    <mergeCell ref="J3:J10"/>
-    <mergeCell ref="J12:J16"/>
-    <mergeCell ref="J18:J22"/>
-    <mergeCell ref="J24:J28"/>
-    <mergeCell ref="J31:J38"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
corrected devis and DMP save operation
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DC843-76CB-4BAC-BE21-FF7AAC012462}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262C515E-775D-43FB-857F-E6A0CB9D1E9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>Export différenciée des devis et DMPs en titrant la colonne "Devis XX" ou "DMP XX"</t>
   </si>
 </sst>
 </file>
@@ -614,8 +617,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="C1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H56" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView tabSelected="1" topLeftCell="G61" workbookViewId="0">
+      <selection activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1098,7 @@
       </c>
       <c r="L47">
         <f>L48+L57+L63+L69+L76+L86</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="10:12" x14ac:dyDescent="0.3">
@@ -1211,7 +1214,7 @@
       </c>
       <c r="L76">
         <f>SUM(L77:L83)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="10:12" x14ac:dyDescent="0.3">
@@ -1234,6 +1237,12 @@
     </row>
     <row r="79" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J79" s="3"/>
+      <c r="K79" t="s">
+        <v>58</v>
+      </c>
+      <c r="L79">
+        <v>4</v>
+      </c>
     </row>
     <row r="80" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J80" s="3"/>
@@ -1256,7 +1265,7 @@
     <row r="86" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J86" s="3"/>
       <c r="K86" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="L86">
         <v>2</v>

</xml_diff>

<commit_message>
cleaned code before implementing sub function to factorise it
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262C515E-775D-43FB-857F-E6A0CB9D1E9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4407EC3-160A-4600-86AE-3B6D5CA5B43F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -192,12 +192,6 @@
     <t>Semaine du 05 au 11 Avril 2021</t>
   </si>
   <si>
-    <t>Semaine du 12 au 19 Avril 2021</t>
-  </si>
-  <si>
-    <t>Numéro de facture</t>
-  </si>
-  <si>
     <t>Validation de facture: sauvegarde des infos du client en gérant les cas où le formulaire serait modifié, enrichi ou appauvri</t>
   </si>
   <si>
@@ -207,10 +201,55 @@
     <t>Affectation d'un bouton dédié pour mettre à jour le calcul de la taxe d'ameublement si besoin</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>Export différenciée des devis et DMPs en titrant la colonne "Devis XX" ou "DMP XX"</t>
+  </si>
+  <si>
+    <t>Ecrasement du numéro de facture lorsque l'utilisateur clique sur le bouton d'impression</t>
+  </si>
+  <si>
+    <t>Semaine du 12 au 18 Avril 2021</t>
+  </si>
+  <si>
+    <t>Montant facture HT</t>
+  </si>
+  <si>
+    <t>Montants TVA N, R, A</t>
+  </si>
+  <si>
+    <t>Factures d'acompte</t>
+  </si>
+  <si>
+    <t>Montant restant dû</t>
+  </si>
+  <si>
+    <t>Montant du marché non encore appelé</t>
+  </si>
+  <si>
+    <t>Contrat CDI, autre contrat (consultant par exemple)</t>
+  </si>
+  <si>
+    <t>Apporteur d'affaire (chèques de garanties pontuels à ne pas encaisser)</t>
+  </si>
+  <si>
+    <t>Adresse de facturation et d'installation</t>
+  </si>
+  <si>
+    <t>Adresse de facturation =&gt; adresse d'installation différente requise</t>
+  </si>
+  <si>
+    <t>Montant HT par typologie de client</t>
+  </si>
+  <si>
+    <t>Semaine du 19 au 25 Avril 2021</t>
+  </si>
+  <si>
+    <t>Créer une fonction prenant en entrée rangeIn et qui va écrire dans l'export</t>
+  </si>
+  <si>
+    <t>Affichage de l'apercu avant impression au clic sur le bouton prévu à cet effet</t>
+  </si>
+  <si>
+    <t>Eléments de la facture à sauvegader</t>
   </si>
 </sst>
 </file>
@@ -220,7 +259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +297,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -285,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -300,6 +346,19 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="120"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="105"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="105"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="95"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,11 +673,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FAB82E3-EF02-4AF5-BC7B-4E3EB2A167A6}">
-  <sheetPr codeName="Feuil1"/>
-  <dimension ref="C1:L89"/>
+  <sheetPr codeName="Feuil1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="C1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G61" workbookViewId="0">
-      <selection activeCell="L86" sqref="L86"/>
+    <sheetView tabSelected="1" topLeftCell="F133" workbookViewId="0">
+      <selection activeCell="K164" sqref="K164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,7 +693,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="1">
-        <f>SUM(D3:D1500)</f>
+        <f>SUM(D3:D1482)</f>
         <v>36.375</v>
       </c>
     </row>
@@ -1094,208 +1155,565 @@
     </row>
     <row r="47" spans="10:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="K47" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L47">
+        <f>L49+L53+L57+L60+L64+L71+L74</f>
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="48" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J48" s="6">
+        <v>44298</v>
+      </c>
+    </row>
+    <row r="49" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J49" s="6"/>
+      <c r="K49" t="s">
         <v>52</v>
-      </c>
-      <c r="L47">
-        <f>L48+L57+L63+L69+L76+L86</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J48" s="4">
-        <v>44298</v>
-      </c>
-    </row>
-    <row r="49" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J49" s="4"/>
-      <c r="K49" t="s">
-        <v>54</v>
       </c>
       <c r="L49">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J50" s="4"/>
+      <c r="J50" s="6"/>
       <c r="K50" t="s">
+        <v>56</v>
+      </c>
+      <c r="L50">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J52" s="7"/>
+    </row>
+    <row r="53" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J53" s="8">
+        <v>44299</v>
+      </c>
+      <c r="L53">
+        <f>SUM(L54:L55)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J54" s="8"/>
+      <c r="K54" t="s">
+        <v>52</v>
+      </c>
+      <c r="L54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J55" s="8"/>
+    </row>
+    <row r="56" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J56" s="7"/>
+    </row>
+    <row r="57" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J57" s="9">
+        <f>J53+1</f>
+        <v>44300</v>
+      </c>
+      <c r="L57">
+        <f>SUM(L58:L58)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J58" s="9"/>
+    </row>
+    <row r="59" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J59" s="7"/>
+    </row>
+    <row r="60" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J60" s="9">
+        <f>J57+1</f>
+        <v>44301</v>
+      </c>
+      <c r="L60">
+        <f>SUM(L61:L61)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J61" s="9"/>
+    </row>
+    <row r="62" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J62" s="7"/>
+    </row>
+    <row r="63" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J63" s="7"/>
+    </row>
+    <row r="64" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J64" s="6">
+        <f>J60+1</f>
+        <v>44302</v>
+      </c>
+      <c r="L64">
+        <f>SUM(L65:L68)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="65" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J65" s="6"/>
+      <c r="K65" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J51" s="4"/>
-    </row>
-    <row r="52" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J54" s="4"/>
-    </row>
-    <row r="55" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J55" s="4"/>
-    </row>
-    <row r="57" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J57" s="5">
-        <v>44299</v>
-      </c>
-      <c r="L57">
-        <f>SUM(L58:L61)</f>
+      <c r="L65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J66" s="6"/>
+      <c r="K66" t="s">
+        <v>54</v>
+      </c>
+      <c r="L66">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J67" s="6"/>
+      <c r="K67" t="s">
+        <v>55</v>
+      </c>
+      <c r="L67">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J58" s="5"/>
-      <c r="K58" t="s">
-        <v>54</v>
-      </c>
-      <c r="L58">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J60" s="5"/>
-    </row>
-    <row r="61" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J61" s="5"/>
-    </row>
-    <row r="63" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J63" s="5">
-        <f>J57+1</f>
-        <v>44300</v>
-      </c>
-      <c r="L63">
-        <f>SUM(L64:L67)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J67" s="5"/>
-    </row>
-    <row r="69" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J69" s="5">
-        <f>J63+1</f>
-        <v>44301</v>
-      </c>
-      <c r="L69">
-        <f>SUM(L70:L72)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J70" s="5"/>
+    <row r="68" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J68" s="6"/>
+    </row>
+    <row r="69" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J69" s="7"/>
+    </row>
+    <row r="70" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J70" s="8">
+        <f>J64+1</f>
+        <v>44303</v>
+      </c>
     </row>
     <row r="71" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J71" s="5"/>
+      <c r="J71" s="8"/>
+      <c r="K71" t="s">
+        <v>55</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
     </row>
     <row r="72" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J72" s="5"/>
+      <c r="J72" s="8"/>
     </row>
     <row r="73" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J73" s="5"/>
+      <c r="J73" s="7"/>
+    </row>
+    <row r="74" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J74" s="6">
+        <f>J70+1</f>
+        <v>44304</v>
+      </c>
+      <c r="L74">
+        <f>SUM(L75:L77)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J75" s="6"/>
+      <c r="K75" t="s">
+        <v>55</v>
+      </c>
+      <c r="L75">
+        <v>2</v>
+      </c>
     </row>
     <row r="76" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J76" s="3">
-        <f>J69+1</f>
-        <v>44302</v>
+      <c r="J76" s="6"/>
+      <c r="K76" t="s">
+        <v>50</v>
       </c>
       <c r="L76">
-        <f>SUM(L77:L83)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J77" s="6"/>
+    </row>
+    <row r="80" spans="10:12" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K80" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L80">
+        <f>L81+L90+L96+L102+L109+L119+L124</f>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="81" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J81" s="4">
+        <v>44305</v>
+      </c>
+      <c r="L81">
+        <f>SUM(L82:L88)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="82" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J82" s="4"/>
+      <c r="L82">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="83" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J83" s="4"/>
+      <c r="L83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J84" s="4"/>
+      <c r="L84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J85" s="4"/>
+      <c r="L85">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J86" s="4"/>
+      <c r="L86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J87" s="4"/>
+      <c r="L87">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J88" s="4"/>
+      <c r="L88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J90" s="5">
+        <f>J81+1</f>
+        <v>44306</v>
+      </c>
+      <c r="L90">
+        <f>SUM(L91:L94)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J91" s="5"/>
+      <c r="L91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J92" s="5"/>
+      <c r="L92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J93" s="5"/>
+      <c r="L93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J94" s="5"/>
+      <c r="L94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J96" s="5">
+        <f>J90+1</f>
+        <v>44307</v>
+      </c>
+      <c r="L96">
+        <f>SUM(L97:L100)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J97" s="5"/>
+      <c r="L97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J98" s="5"/>
+      <c r="L98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J99" s="5"/>
+      <c r="L99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J100" s="5"/>
+      <c r="L100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J102" s="3">
+        <f>J96+1</f>
+        <v>44308</v>
+      </c>
+      <c r="L102">
+        <f>SUM(L103:L105)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J77" s="3"/>
-      <c r="K77" t="s">
-        <v>55</v>
-      </c>
-      <c r="L77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J78" s="3"/>
-      <c r="K78" t="s">
-        <v>56</v>
-      </c>
-      <c r="L78" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="79" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J79" s="3"/>
-      <c r="K79" t="s">
+    <row r="103" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J103" s="3"/>
+      <c r="L103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J104" s="3"/>
+      <c r="L104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J105" s="3"/>
+      <c r="L105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J106" s="3"/>
+    </row>
+    <row r="107" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J109" s="3">
+        <f>J102+1</f>
+        <v>44309</v>
+      </c>
+      <c r="L109">
+        <f>SUM(L110:L116)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J110" s="3"/>
+      <c r="L110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J111" s="3"/>
+      <c r="L111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J112" s="3"/>
+      <c r="L112">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="113" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J113" s="3"/>
+      <c r="L113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J114" s="3"/>
+      <c r="L114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J115" s="3"/>
+      <c r="L115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J116" s="3"/>
+      <c r="L116">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J118" s="3">
+        <f>J109+1</f>
+        <v>44310</v>
+      </c>
+      <c r="L118">
+        <f>SUM(L119:L122)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J119" s="3"/>
+      <c r="L119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J120" s="3"/>
+    </row>
+    <row r="121" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J121" s="3"/>
+    </row>
+    <row r="122" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J122" s="3"/>
+    </row>
+    <row r="124" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J124" s="3">
+        <f>J118+1</f>
+        <v>44311</v>
+      </c>
+      <c r="L124">
+        <f>SUM(L125:L128)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J125" s="3"/>
+      <c r="L125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J126" s="3"/>
+    </row>
+    <row r="127" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J127" s="3"/>
+    </row>
+    <row r="128" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J128" s="3"/>
+    </row>
+    <row r="135" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K135" t="s">
+        <v>70</v>
+      </c>
+      <c r="L135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K136" t="s">
+        <v>69</v>
+      </c>
+      <c r="L136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L137" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="138" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L138" t="s">
         <v>58</v>
       </c>
-      <c r="L79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J80" s="3"/>
-    </row>
-    <row r="81" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J82" s="3"/>
-    </row>
-    <row r="83" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J83" s="3"/>
-    </row>
-    <row r="85" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J85" s="3">
-        <f>J76+1</f>
-        <v>44303</v>
-      </c>
-    </row>
-    <row r="86" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J86" s="3"/>
-      <c r="K86" t="s">
-        <v>58</v>
-      </c>
-      <c r="L86">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J87" s="3"/>
-    </row>
-    <row r="88" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J88" s="3"/>
-    </row>
-    <row r="89" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J89" s="3"/>
+    </row>
+    <row r="139" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L139" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="140" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L140" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="141" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L141" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L142" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="143" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L143" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="144" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K144" s="10"/>
+    </row>
+    <row r="156" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K156" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="157" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K157" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="160" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K160" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="161" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K161" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
+    <mergeCell ref="J81:J88"/>
+    <mergeCell ref="J90:J94"/>
+    <mergeCell ref="J96:J100"/>
+    <mergeCell ref="J102:J106"/>
+    <mergeCell ref="J109:J116"/>
+    <mergeCell ref="J118:J122"/>
+    <mergeCell ref="J124:J128"/>
+    <mergeCell ref="J74:J77"/>
     <mergeCell ref="J3:J10"/>
     <mergeCell ref="J12:J16"/>
     <mergeCell ref="J18:J22"/>
     <mergeCell ref="J24:J28"/>
     <mergeCell ref="J31:J38"/>
-    <mergeCell ref="J76:J83"/>
-    <mergeCell ref="J85:J89"/>
+    <mergeCell ref="J64:J68"/>
+    <mergeCell ref="J70:J72"/>
     <mergeCell ref="J40:J44"/>
-    <mergeCell ref="J48:J55"/>
-    <mergeCell ref="J57:J61"/>
-    <mergeCell ref="J63:J67"/>
-    <mergeCell ref="J69:J73"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="J53:J55"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="J60:J61"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.8" footer="0.8"/>
+  <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C&amp;"Raleway,Normal"
+SAS Technipose Solomas France ZI La Vallière - 06730 SAINT ANDRE DE LA ROCHE - SIRET 421 611 096 00023
+N° de T.V.A FR 54421611096&amp;R&amp;"Raleway,Gras"Page &amp;P de &amp;N
+</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
managed client infos with common export function
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4407EC3-160A-4600-86AE-3B6D5CA5B43F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC32DD9-7DBF-4337-955B-868FD8BF609D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Eléments de la facture à sauvegader</t>
+  </si>
+  <si>
+    <t>Faire une structure pour ClientDetails pour fiter rangeIn</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -359,6 +362,7 @@
       <alignment horizontal="center" vertical="center" textRotation="95"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,12 +678,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FAB82E3-EF02-4AF5-BC7B-4E3EB2A167A6}">
   <sheetPr codeName="Feuil1">
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="C1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F133" workbookViewId="0">
-      <selection activeCell="K164" sqref="K164"/>
+    <sheetView tabSelected="1" topLeftCell="F102" workbookViewId="0">
+      <selection activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1351,59 +1355,46 @@
       </c>
       <c r="L80">
         <f>L81+L90+L96+L102+L109+L119+L124</f>
-        <v>40.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J81" s="4">
         <v>44305</v>
       </c>
+      <c r="K81" t="s">
+        <v>70</v>
+      </c>
       <c r="L81">
-        <f>SUM(L82:L88)</f>
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J82" s="4"/>
+      <c r="K82" t="s">
+        <v>69</v>
+      </c>
       <c r="L82">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J83" s="4"/>
-      <c r="L83">
-        <v>1</v>
-      </c>
     </row>
     <row r="84" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J84" s="4"/>
-      <c r="L84">
-        <v>1</v>
-      </c>
     </row>
     <row r="85" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J85" s="4"/>
-      <c r="L85">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="86" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J86" s="4"/>
-      <c r="L86">
-        <v>1</v>
-      </c>
     </row>
     <row r="87" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J87" s="4"/>
-      <c r="L87">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="88" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J88" s="4"/>
-      <c r="L88">
-        <v>2</v>
-      </c>
     </row>
     <row r="90" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J90" s="5">
@@ -1412,32 +1403,26 @@
       </c>
       <c r="L90">
         <f>SUM(L91:L94)</f>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J91" s="5"/>
+      <c r="K91" t="s">
+        <v>69</v>
+      </c>
       <c r="L91">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J92" s="5"/>
-      <c r="L92">
-        <v>2</v>
-      </c>
     </row>
     <row r="93" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J93" s="5"/>
-      <c r="L93">
-        <v>3</v>
-      </c>
     </row>
     <row r="94" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J94" s="5"/>
-      <c r="L94">
-        <v>2</v>
-      </c>
     </row>
     <row r="96" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J96" s="5">
@@ -1446,34 +1431,25 @@
       </c>
       <c r="L96">
         <f>SUM(L97:L100)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="10:12" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J97" s="5"/>
-      <c r="L97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K97" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J98" s="5"/>
-      <c r="L98">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J99" s="5"/>
-      <c r="L99">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J100" s="5"/>
-      <c r="L100">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J102" s="3">
         <f>J96+1</f>
         <v>44308</v>
@@ -1483,80 +1459,66 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J103" s="3"/>
       <c r="L103">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J104" s="3"/>
       <c r="L104">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J105" s="3"/>
       <c r="L105">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J109" s="3">
         <f>J102+1</f>
         <v>44309</v>
       </c>
       <c r="L109">
         <f>SUM(L110:L116)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="110" spans="10:12" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="H110" s="11"/>
       <c r="J110" s="3"/>
+      <c r="K110" t="s">
+        <v>72</v>
+      </c>
       <c r="L110">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="10:12" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J111" s="3"/>
-      <c r="L111">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="10:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="8:12" x14ac:dyDescent="0.3">
       <c r="J112" s="3"/>
-      <c r="L112">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="113" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J113" s="3"/>
-      <c r="L113">
-        <v>1</v>
-      </c>
     </row>
     <row r="114" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J114" s="3"/>
-      <c r="L114">
-        <v>1</v>
-      </c>
     </row>
     <row r="115" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J115" s="3"/>
-      <c r="L115">
-        <v>1</v>
-      </c>
     </row>
     <row r="116" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J116" s="3"/>
-      <c r="L116">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="118" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J118" s="3">

</xml_diff>

<commit_message>
managed typlogie client, social networks, review and check montants devis
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC32DD9-7DBF-4337-955B-868FD8BF609D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F7DD2B-C89D-41B7-90D6-9AEF1E3D1968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -252,7 +252,31 @@
     <t>Eléments de la facture à sauvegader</t>
   </si>
   <si>
-    <t>Faire une structure pour ClientDetails pour fiter rangeIn</t>
+    <t>Faire une structure pour ClientDetails pour s'adapter à la structure de rangeIn</t>
+  </si>
+  <si>
+    <t>Export des Devis et DMPs: construction des structures de type rangeIn</t>
+  </si>
+  <si>
+    <t>Export des Devis et DMPs: appel à la méthode générique exportReferencesFromRange</t>
+  </si>
+  <si>
+    <t>Export des Devis et DMPs: adaptation de la méthode exportReferencesFromRange pour la faire marcher avec l'input</t>
+  </si>
+  <si>
+    <t>Client and invoice identification: adapter l'algo pour reproduire la mise en forme ligne - 2</t>
+  </si>
+  <si>
+    <t>Ajout de la typologie client</t>
+  </si>
+  <si>
+    <t>Typologie Client</t>
+  </si>
+  <si>
+    <t>Ajout d'un encart réseaux sociaux en page de récap</t>
+  </si>
+  <si>
+    <t>Mise en place de "Votre avis compte"</t>
   </si>
 </sst>
 </file>
@@ -683,7 +707,7 @@
   <dimension ref="C1:L161"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F102" workbookViewId="0">
-      <selection activeCell="K111" sqref="K111"/>
+      <selection activeCell="L123" sqref="L123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,7 +1379,7 @@
       </c>
       <c r="L80">
         <f>L81+L90+L96+L102+L109+L119+L124</f>
-        <v>13</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="81" spans="10:12" x14ac:dyDescent="0.3">
@@ -1434,22 +1458,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J97" s="5"/>
       <c r="K97" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J100" s="5"/>
     </row>
-    <row r="102" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J102" s="3">
         <f>J96+1</f>
         <v>44308</v>
@@ -1459,40 +1483,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J103" s="3"/>
       <c r="L103">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J104" s="3"/>
       <c r="L104">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J105" s="3"/>
       <c r="L105">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="8:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F107" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="108" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F108" s="11">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G108" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J109" s="3">
         <f>J102+1</f>
         <v>44309</v>
       </c>
       <c r="L109">
         <f>SUM(L110:L116)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="110" spans="8:12" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="6:12" x14ac:dyDescent="0.3">
       <c r="H110" s="11"/>
       <c r="J110" s="3"/>
       <c r="K110" t="s">
@@ -1502,14 +1537,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J111" s="3"/>
-    </row>
-    <row r="112" spans="8:12" x14ac:dyDescent="0.3">
+      <c r="K111" t="s">
+        <v>73</v>
+      </c>
+      <c r="L111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J112" s="3"/>
+      <c r="K112" t="s">
+        <v>74</v>
+      </c>
+      <c r="L112">
+        <v>1</v>
+      </c>
     </row>
     <row r="113" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J113" s="3"/>
+      <c r="K113" t="s">
+        <v>75</v>
+      </c>
+      <c r="L113">
+        <v>4</v>
+      </c>
     </row>
     <row r="114" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J114" s="3"/>
@@ -1527,23 +1580,44 @@
       </c>
       <c r="L118">
         <f>SUM(L119:L122)</f>
-        <v>2</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="119" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J119" s="3"/>
+      <c r="K119" t="s">
+        <v>76</v>
+      </c>
       <c r="L119">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="120" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J120" s="3"/>
+      <c r="K120" t="s">
+        <v>77</v>
+      </c>
+      <c r="L120">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="121" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J121" s="3"/>
+      <c r="K121" t="s">
+        <v>79</v>
+      </c>
+      <c r="L121">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="122" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J122" s="3"/>
+      <c r="K122" t="s">
+        <v>80</v>
+      </c>
+      <c r="L122">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="124" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J124" s="3">
@@ -1623,6 +1697,9 @@
     </row>
     <row r="144" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K144" s="10"/>
+      <c r="L144" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="156" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K156" t="s">

</xml_diff>

<commit_message>
implemented new invoice and new facturier
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F7DD2B-C89D-41B7-90D6-9AEF1E3D1968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A466EA-7414-4E67-BBBC-72045D551496}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
+    <workbookView xWindow="40350" yWindow="5340" windowWidth="17280" windowHeight="10050" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -277,6 +276,21 @@
   </si>
   <si>
     <t>Mise en place de "Votre avis compte"</t>
+  </si>
+  <si>
+    <t>Mise en place du check que le montant TTC d'un devis correspond à ce qui est annoncé</t>
+  </si>
+  <si>
+    <t>Ajout d'une ligne à l'impression des titres (esthétique)</t>
+  </si>
+  <si>
+    <t>Suppression de toutes les références à template en trop dans le code</t>
+  </si>
+  <si>
+    <t>Bouton nouvelle facture et implémentation de l'algo chargé de figer le numéro de la facture sur laquelle on travaille si ce n'est pas le template et de créer avant la feuille informations enregistrées une nouvelle facture dont le nom est choisi par l'utilisateur</t>
+  </si>
+  <si>
+    <t>Bouton nouveau facturier avec nom du mois pré-rempli et check global qui regarde si on travaille avec le bon facturier</t>
   </si>
 </sst>
 </file>
@@ -364,8 +378,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="120"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="105"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="120"/>
@@ -373,20 +395,12 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="120"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="105"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="105"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="95"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,8 +720,8 @@
   </sheetPr>
   <dimension ref="C1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F102" workbookViewId="0">
-      <selection activeCell="L123" sqref="L123"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +758,7 @@
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="8">
         <v>44292</v>
       </c>
       <c r="L3">
@@ -762,7 +776,7 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="8"/>
       <c r="K4" t="s">
         <v>25</v>
       </c>
@@ -777,7 +791,7 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="8"/>
       <c r="K5" t="s">
         <v>26</v>
       </c>
@@ -792,7 +806,7 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="8"/>
       <c r="K6" t="s">
         <v>46</v>
       </c>
@@ -807,7 +821,7 @@
       <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="8"/>
       <c r="K7" t="s">
         <v>27</v>
       </c>
@@ -822,7 +836,7 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="8"/>
       <c r="K8" t="s">
         <v>28</v>
       </c>
@@ -840,7 +854,7 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="8"/>
       <c r="K9" t="s">
         <v>48</v>
       </c>
@@ -855,7 +869,7 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="8"/>
       <c r="K10" t="s">
         <v>47</v>
       </c>
@@ -878,7 +892,7 @@
       <c r="E12" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="9">
         <v>44293</v>
       </c>
       <c r="L12">
@@ -887,7 +901,7 @@
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J13" s="5"/>
+      <c r="J13" s="9"/>
       <c r="K13" t="s">
         <v>29</v>
       </c>
@@ -905,7 +919,7 @@
       <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="9"/>
       <c r="K14" t="s">
         <v>30</v>
       </c>
@@ -914,7 +928,7 @@
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J15" s="5"/>
+      <c r="J15" s="9"/>
       <c r="K15" t="s">
         <v>31</v>
       </c>
@@ -932,7 +946,7 @@
       <c r="E16" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16" s="9"/>
       <c r="K16" t="s">
         <v>32</v>
       </c>
@@ -950,7 +964,7 @@
       <c r="E18" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="9">
         <v>44294</v>
       </c>
       <c r="L18">
@@ -965,7 +979,7 @@
       <c r="E19" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="5"/>
+      <c r="J19" s="9"/>
       <c r="K19" t="s">
         <v>33</v>
       </c>
@@ -983,7 +997,7 @@
       <c r="E20" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="J20" s="9"/>
       <c r="K20" t="s">
         <v>37</v>
       </c>
@@ -998,7 +1012,7 @@
       <c r="E21" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="J21" s="9"/>
       <c r="K21" t="s">
         <v>34</v>
       </c>
@@ -1007,7 +1021,7 @@
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J22" s="5"/>
+      <c r="J22" s="9"/>
       <c r="K22" t="s">
         <v>35</v>
       </c>
@@ -1030,7 +1044,7 @@
       <c r="E24" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="6">
         <v>44295</v>
       </c>
       <c r="L24">
@@ -1039,7 +1053,7 @@
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J25" s="3"/>
+      <c r="J25" s="6"/>
       <c r="K25" t="s">
         <v>39</v>
       </c>
@@ -1057,7 +1071,7 @@
       <c r="E26" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="3"/>
+      <c r="J26" s="6"/>
       <c r="K26" t="s">
         <v>36</v>
       </c>
@@ -1072,7 +1086,7 @@
       <c r="E27" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="3"/>
+      <c r="J27" s="6"/>
       <c r="K27" t="s">
         <v>38</v>
       </c>
@@ -1081,13 +1095,13 @@
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J28" s="3"/>
+      <c r="J28" s="6"/>
       <c r="K28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J31" s="3">
+      <c r="J31" s="6">
         <v>44296</v>
       </c>
       <c r="L31">
@@ -1096,7 +1110,7 @@
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="J32" s="3"/>
+      <c r="J32" s="6"/>
       <c r="K32" t="s">
         <v>39</v>
       </c>
@@ -1105,7 +1119,7 @@
       </c>
     </row>
     <row r="33" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J33" s="3"/>
+      <c r="J33" s="6"/>
       <c r="K33" t="s">
         <v>40</v>
       </c>
@@ -1114,7 +1128,7 @@
       </c>
     </row>
     <row r="34" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J34" s="3"/>
+      <c r="J34" s="6"/>
       <c r="K34" t="s">
         <v>41</v>
       </c>
@@ -1123,7 +1137,7 @@
       </c>
     </row>
     <row r="35" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J35" s="3"/>
+      <c r="J35" s="6"/>
       <c r="K35" t="s">
         <v>42</v>
       </c>
@@ -1132,7 +1146,7 @@
       </c>
     </row>
     <row r="36" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J36" s="3"/>
+      <c r="J36" s="6"/>
       <c r="K36" t="s">
         <v>43</v>
       </c>
@@ -1141,7 +1155,7 @@
       </c>
     </row>
     <row r="37" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J37" s="3"/>
+      <c r="J37" s="6"/>
       <c r="K37" t="s">
         <v>44</v>
       </c>
@@ -1150,7 +1164,7 @@
       </c>
     </row>
     <row r="38" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J38" s="3"/>
+      <c r="J38" s="6"/>
       <c r="K38" t="s">
         <v>45</v>
       </c>
@@ -1159,12 +1173,12 @@
       </c>
     </row>
     <row r="40" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J40" s="3">
+      <c r="J40" s="6">
         <v>44297</v>
       </c>
     </row>
     <row r="41" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J41" s="3"/>
+      <c r="J41" s="6"/>
       <c r="K41" t="s">
         <v>50</v>
       </c>
@@ -1173,13 +1187,13 @@
       </c>
     </row>
     <row r="42" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J42" s="3"/>
+      <c r="J42" s="6"/>
     </row>
     <row r="43" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J43" s="3"/>
+      <c r="J43" s="6"/>
     </row>
     <row r="44" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J44" s="3"/>
+      <c r="J44" s="6"/>
     </row>
     <row r="47" spans="10:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="K47" s="2" t="s">
@@ -1191,12 +1205,12 @@
       </c>
     </row>
     <row r="48" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J48" s="6">
+      <c r="J48" s="7">
         <v>44298</v>
       </c>
     </row>
     <row r="49" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J49" s="6"/>
+      <c r="J49" s="7"/>
       <c r="K49" t="s">
         <v>52</v>
       </c>
@@ -1205,7 +1219,7 @@
       </c>
     </row>
     <row r="50" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J50" s="6"/>
+      <c r="J50" s="7"/>
       <c r="K50" t="s">
         <v>56</v>
       </c>
@@ -1214,13 +1228,13 @@
       </c>
     </row>
     <row r="51" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J51" s="6"/>
+      <c r="J51" s="7"/>
     </row>
     <row r="52" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J52" s="7"/>
+      <c r="J52" s="3"/>
     </row>
     <row r="53" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J53" s="8">
+      <c r="J53" s="10">
         <v>44299</v>
       </c>
       <c r="L53">
@@ -1229,7 +1243,7 @@
       </c>
     </row>
     <row r="54" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J54" s="8"/>
+      <c r="J54" s="10"/>
       <c r="K54" t="s">
         <v>52</v>
       </c>
@@ -1238,13 +1252,13 @@
       </c>
     </row>
     <row r="55" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J55" s="8"/>
+      <c r="J55" s="10"/>
     </row>
     <row r="56" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J56" s="7"/>
+      <c r="J56" s="3"/>
     </row>
     <row r="57" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J57" s="9">
+      <c r="J57" s="11">
         <f>J53+1</f>
         <v>44300</v>
       </c>
@@ -1254,13 +1268,13 @@
       </c>
     </row>
     <row r="58" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J58" s="9"/>
+      <c r="J58" s="11"/>
     </row>
     <row r="59" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J59" s="7"/>
+      <c r="J59" s="3"/>
     </row>
     <row r="60" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J60" s="9">
+      <c r="J60" s="11">
         <f>J57+1</f>
         <v>44301</v>
       </c>
@@ -1270,16 +1284,16 @@
       </c>
     </row>
     <row r="61" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J61" s="9"/>
+      <c r="J61" s="11"/>
     </row>
     <row r="62" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J62" s="7"/>
+      <c r="J62" s="3"/>
     </row>
     <row r="63" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J63" s="7"/>
+      <c r="J63" s="3"/>
     </row>
     <row r="64" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J64" s="6">
+      <c r="J64" s="7">
         <f>J60+1</f>
         <v>44302</v>
       </c>
@@ -1289,7 +1303,7 @@
       </c>
     </row>
     <row r="65" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J65" s="6"/>
+      <c r="J65" s="7"/>
       <c r="K65" t="s">
         <v>53</v>
       </c>
@@ -1298,7 +1312,7 @@
       </c>
     </row>
     <row r="66" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J66" s="6"/>
+      <c r="J66" s="7"/>
       <c r="K66" t="s">
         <v>54</v>
       </c>
@@ -1307,7 +1321,7 @@
       </c>
     </row>
     <row r="67" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J67" s="6"/>
+      <c r="J67" s="7"/>
       <c r="K67" t="s">
         <v>55</v>
       </c>
@@ -1316,19 +1330,19 @@
       </c>
     </row>
     <row r="68" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J68" s="6"/>
+      <c r="J68" s="7"/>
     </row>
     <row r="69" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J69" s="7"/>
+      <c r="J69" s="3"/>
     </row>
     <row r="70" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J70" s="8">
+      <c r="J70" s="10">
         <f>J64+1</f>
         <v>44303</v>
       </c>
     </row>
     <row r="71" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J71" s="8"/>
+      <c r="J71" s="10"/>
       <c r="K71" t="s">
         <v>55</v>
       </c>
@@ -1337,13 +1351,13 @@
       </c>
     </row>
     <row r="72" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J72" s="8"/>
+      <c r="J72" s="10"/>
     </row>
     <row r="73" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J73" s="7"/>
+      <c r="J73" s="3"/>
     </row>
     <row r="74" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J74" s="6">
+      <c r="J74" s="7">
         <f>J70+1</f>
         <v>44304</v>
       </c>
@@ -1353,7 +1367,7 @@
       </c>
     </row>
     <row r="75" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J75" s="6"/>
+      <c r="J75" s="7"/>
       <c r="K75" t="s">
         <v>55</v>
       </c>
@@ -1362,7 +1376,7 @@
       </c>
     </row>
     <row r="76" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J76" s="6"/>
+      <c r="J76" s="7"/>
       <c r="K76" t="s">
         <v>50</v>
       </c>
@@ -1371,7 +1385,7 @@
       </c>
     </row>
     <row r="77" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J77" s="6"/>
+      <c r="J77" s="7"/>
     </row>
     <row r="80" spans="10:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="K80" s="2" t="s">
@@ -1379,11 +1393,11 @@
       </c>
       <c r="L80">
         <f>L81+L90+L96+L102+L109+L119+L124</f>
-        <v>18.5</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="81" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J81" s="4">
+      <c r="J81" s="8">
         <v>44305</v>
       </c>
       <c r="K81" t="s">
@@ -1394,7 +1408,7 @@
       </c>
     </row>
     <row r="82" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J82" s="4"/>
+      <c r="J82" s="8"/>
       <c r="K82" t="s">
         <v>69</v>
       </c>
@@ -1403,25 +1417,25 @@
       </c>
     </row>
     <row r="83" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J83" s="4"/>
+      <c r="J83" s="8"/>
     </row>
     <row r="84" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J84" s="4"/>
+      <c r="J84" s="8"/>
     </row>
     <row r="85" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J85" s="4"/>
+      <c r="J85" s="8"/>
     </row>
     <row r="86" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J86" s="4"/>
+      <c r="J86" s="8"/>
     </row>
     <row r="87" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J87" s="4"/>
+      <c r="J87" s="8"/>
     </row>
     <row r="88" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J88" s="4"/>
+      <c r="J88" s="8"/>
     </row>
     <row r="90" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J90" s="5">
+      <c r="J90" s="9">
         <f>J81+1</f>
         <v>44306</v>
       </c>
@@ -1431,7 +1445,7 @@
       </c>
     </row>
     <row r="91" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J91" s="5"/>
+      <c r="J91" s="9"/>
       <c r="K91" t="s">
         <v>69</v>
       </c>
@@ -1440,41 +1454,47 @@
       </c>
     </row>
     <row r="92" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J92" s="5"/>
+      <c r="J92" s="9"/>
     </row>
     <row r="93" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J93" s="5"/>
+      <c r="J93" s="9"/>
     </row>
     <row r="94" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J94" s="5"/>
+      <c r="J94" s="9"/>
     </row>
     <row r="96" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J96" s="5">
+      <c r="J96" s="9">
         <f>J90+1</f>
         <v>44307</v>
       </c>
       <c r="L96">
         <f>SUM(L97:L100)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="97" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J97" s="5"/>
+      <c r="J97" s="9"/>
       <c r="K97" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="98" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J98" s="5"/>
+      <c r="J98" s="9"/>
+      <c r="K98" t="s">
+        <v>82</v>
+      </c>
+      <c r="L98">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="99" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J99" s="5"/>
+      <c r="J99" s="9"/>
     </row>
     <row r="100" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J100" s="5"/>
+      <c r="J100" s="9"/>
     </row>
     <row r="102" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J102" s="3">
+      <c r="J102" s="6">
         <f>J96+1</f>
         <v>44308</v>
       </c>
@@ -1484,41 +1504,42 @@
       </c>
     </row>
     <row r="103" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J103" s="3"/>
+      <c r="J103" s="6"/>
       <c r="L103">
         <v>2</v>
       </c>
     </row>
     <row r="104" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J104" s="3"/>
+      <c r="J104" s="6"/>
       <c r="L104">
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J105" s="3"/>
+      <c r="J105" s="6"/>
       <c r="L105">
         <v>2</v>
       </c>
     </row>
     <row r="106" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J106" s="3"/>
+      <c r="F106" s="5"/>
+      <c r="J106" s="6"/>
     </row>
     <row r="107" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F107" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="108" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F108" s="11">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="G108" s="11">
-        <v>0</v>
+      <c r="F108" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G108" s="5">
+        <v>0.1875</v>
       </c>
     </row>
     <row r="109" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J109" s="3">
+      <c r="J109" s="6">
         <f>J102+1</f>
         <v>44309</v>
       </c>
@@ -1528,8 +1549,8 @@
       </c>
     </row>
     <row r="110" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="H110" s="11"/>
-      <c r="J110" s="3"/>
+      <c r="H110" s="5"/>
+      <c r="J110" s="6"/>
       <c r="K110" t="s">
         <v>72</v>
       </c>
@@ -1538,7 +1559,7 @@
       </c>
     </row>
     <row r="111" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J111" s="3"/>
+      <c r="J111" s="6"/>
       <c r="K111" t="s">
         <v>73</v>
       </c>
@@ -1547,7 +1568,7 @@
       </c>
     </row>
     <row r="112" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J112" s="3"/>
+      <c r="J112" s="6"/>
       <c r="K112" t="s">
         <v>74</v>
       </c>
@@ -1556,7 +1577,7 @@
       </c>
     </row>
     <row r="113" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J113" s="3"/>
+      <c r="J113" s="6"/>
       <c r="K113" t="s">
         <v>75</v>
       </c>
@@ -1565,26 +1586,26 @@
       </c>
     </row>
     <row r="114" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J114" s="3"/>
+      <c r="J114" s="6"/>
     </row>
     <row r="115" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J115" s="3"/>
+      <c r="J115" s="6"/>
     </row>
     <row r="116" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J116" s="3"/>
+      <c r="J116" s="6"/>
     </row>
     <row r="118" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J118" s="3">
+      <c r="J118" s="6">
         <f>J109+1</f>
         <v>44310</v>
       </c>
       <c r="L118">
-        <f>SUM(L119:L122)</f>
-        <v>1.25</v>
+        <f>SUM(L119:L123)</f>
+        <v>3.25</v>
       </c>
     </row>
     <row r="119" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J119" s="3"/>
+      <c r="J119" s="6"/>
       <c r="K119" t="s">
         <v>76</v>
       </c>
@@ -1593,7 +1614,7 @@
       </c>
     </row>
     <row r="120" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J120" s="3"/>
+      <c r="J120" s="6"/>
       <c r="K120" t="s">
         <v>77</v>
       </c>
@@ -1602,7 +1623,7 @@
       </c>
     </row>
     <row r="121" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J121" s="3"/>
+      <c r="J121" s="6"/>
       <c r="K121" t="s">
         <v>79</v>
       </c>
@@ -1611,7 +1632,7 @@
       </c>
     </row>
     <row r="122" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J122" s="3"/>
+      <c r="J122" s="6"/>
       <c r="K122" t="s">
         <v>80</v>
       </c>
@@ -1619,8 +1640,16 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="123" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K123" t="s">
+        <v>81</v>
+      </c>
+      <c r="L123">
+        <v>2</v>
+      </c>
+    </row>
     <row r="124" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J124" s="3">
+      <c r="J124" s="6">
         <f>J118+1</f>
         <v>44311</v>
       </c>
@@ -1630,19 +1659,28 @@
       </c>
     </row>
     <row r="125" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J125" s="3"/>
+      <c r="J125" s="6"/>
+      <c r="K125" t="s">
+        <v>83</v>
+      </c>
       <c r="L125">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J126" s="3"/>
+      <c r="J126" s="6"/>
+      <c r="K126" t="s">
+        <v>84</v>
+      </c>
+      <c r="L126">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J127" s="3"/>
+      <c r="J127" s="6"/>
     </row>
     <row r="128" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J128" s="3"/>
+      <c r="J128" s="6"/>
     </row>
     <row r="135" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K135" t="s">
@@ -1691,12 +1729,12 @@
       </c>
     </row>
     <row r="143" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L143" s="10" t="s">
+      <c r="L143" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="144" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K144" s="10"/>
+      <c r="K144" s="4"/>
       <c r="L144" t="s">
         <v>78</v>
       </c>
@@ -1723,7 +1761,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="J81:J88"/>
     <mergeCell ref="J90:J94"/>
     <mergeCell ref="J96:J100"/>
     <mergeCell ref="J102:J106"/>
@@ -1743,6 +1780,7 @@
     <mergeCell ref="J53:J55"/>
     <mergeCell ref="J57:J58"/>
     <mergeCell ref="J60:J61"/>
+    <mergeCell ref="J81:J88"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
corrected he way the ranges were searched on the refreshNamedRanges function
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A466EA-7414-4E67-BBBC-72045D551496}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9C9465-E75F-4E1B-A055-6ACF42DA818A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40350" yWindow="5340" windowWidth="17280" windowHeight="10050" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>Bouton nouveau facturier avec nom du mois pré-rempli et check global qui regarde si on travaille avec le bon facturier</t>
+  </si>
+  <si>
+    <t>Mettre le template d'équere + simulation de création d'une facture</t>
+  </si>
+  <si>
+    <t>Correctif: recherche des bornes des différents ranges pour la vérification globale</t>
   </si>
 </sst>
 </file>
@@ -720,8 +726,8 @@
   </sheetPr>
   <dimension ref="C1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="L130" sqref="L130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1393,7 +1399,7 @@
       </c>
       <c r="L80">
         <f>L81+L90+L96+L102+L109+L119+L124</f>
-        <v>18.75</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="81" spans="10:12" x14ac:dyDescent="0.3">
@@ -1527,7 +1533,7 @@
     </row>
     <row r="107" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F107" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1535,7 +1541,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G108" s="5">
-        <v>0.1875</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="109" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1654,8 +1660,8 @@
         <v>44311</v>
       </c>
       <c r="L124">
-        <f>SUM(L125:L128)</f>
-        <v>2</v>
+        <f>SUM(L125:L130)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="10:12" x14ac:dyDescent="0.3">
@@ -1678,9 +1684,29 @@
     </row>
     <row r="127" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J127" s="6"/>
+      <c r="K127" t="s">
+        <v>85</v>
+      </c>
+      <c r="L127">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J128" s="6"/>
+      <c r="K128" t="s">
+        <v>86</v>
+      </c>
+      <c r="L128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K129" t="s">
+        <v>87</v>
+      </c>
+      <c r="L129">
+        <v>2</v>
+      </c>
     </row>
     <row r="135" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K135" t="s">

</xml_diff>

<commit_message>
few correcctions to the central code
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9C9465-E75F-4E1B-A055-6ACF42DA818A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785ACA16-9AE2-472C-B29A-60AEA1E790DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40350" yWindow="5340" windowWidth="17280" windowHeight="10050" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -297,6 +297,12 @@
   </si>
   <si>
     <t>Correctif: recherche des bornes des différents ranges pour la vérification globale</t>
+  </si>
+  <si>
+    <t>modification des ranges nommées attachées au classeur entier</t>
+  </si>
+  <si>
+    <t>Semaine du 26 Avril au 02 Mai 2021</t>
   </si>
 </sst>
 </file>
@@ -306,7 +312,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +357,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -378,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -407,6 +421,8 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="95"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,10 +740,10 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:L161"/>
+  <dimension ref="C1:L208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="L130" sqref="L130"/>
+    <sheetView tabSelected="1" topLeftCell="D123" workbookViewId="0">
+      <selection activeCell="K139" sqref="K139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +757,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="1">
-        <f>SUM(D3:D1482)</f>
+        <f>SUM(D3:D1480)</f>
         <v>36.375</v>
       </c>
     </row>
@@ -1397,277 +1413,271 @@
       <c r="K80" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L80">
-        <f>L81+L90+L96+L102+L109+L119+L124</f>
-        <v>22.75</v>
+      <c r="L80" s="13">
+        <f>L81+L86+L92+L98+L105+L115+L122</f>
+        <v>24.75</v>
       </c>
     </row>
     <row r="81" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J81" s="8">
+      <c r="J81" s="7">
         <v>44305</v>
       </c>
-      <c r="K81" t="s">
+      <c r="L81">
+        <f>SUM(L82:L84)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J82" s="7"/>
+      <c r="K82" t="s">
         <v>70</v>
       </c>
-      <c r="L81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J82" s="8"/>
-      <c r="K82" t="s">
+      <c r="L82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J83" s="7"/>
+      <c r="K83" t="s">
         <v>69</v>
       </c>
-      <c r="L82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J83" s="8"/>
+      <c r="L83">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J84" s="8"/>
-    </row>
-    <row r="85" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J85" s="8"/>
-    </row>
-    <row r="86" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J86" s="8"/>
-    </row>
-    <row r="87" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J87" s="8"/>
-    </row>
-    <row r="88" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J88" s="8"/>
-    </row>
-    <row r="90" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J90" s="9">
+      <c r="J84" s="7"/>
+    </row>
+    <row r="86" spans="10:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J86" s="7">
         <f>J81+1</f>
         <v>44306</v>
       </c>
-      <c r="L90">
-        <f>SUM(L91:L94)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J91" s="9"/>
-      <c r="K91" t="s">
+      <c r="L86">
+        <f>SUM(L87:L89)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J87" s="7"/>
+      <c r="K87" t="s">
         <v>69</v>
       </c>
-      <c r="L91">
-        <v>1</v>
-      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J88" s="7"/>
+    </row>
+    <row r="89" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J89" s="7"/>
     </row>
     <row r="92" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J92" s="9"/>
+      <c r="J92" s="9">
+        <f>J86+1</f>
+        <v>44307</v>
+      </c>
+      <c r="L92" s="12">
+        <f>SUM(L93:L96)</f>
+        <v>1.25</v>
+      </c>
     </row>
     <row r="93" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J93" s="9"/>
+      <c r="K93" t="s">
+        <v>69</v>
+      </c>
+      <c r="L93">
+        <v>1</v>
+      </c>
     </row>
     <row r="94" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J94" s="9"/>
+      <c r="K94" t="s">
+        <v>82</v>
+      </c>
+      <c r="L94">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="95" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J95" s="9"/>
     </row>
     <row r="96" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J96" s="9">
-        <f>J90+1</f>
-        <v>44307</v>
-      </c>
-      <c r="L96">
-        <f>SUM(L97:L100)</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="97" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J97" s="9"/>
-      <c r="K97" t="s">
-        <v>69</v>
-      </c>
+      <c r="J96" s="9"/>
     </row>
     <row r="98" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J98" s="9"/>
-      <c r="K98" t="s">
-        <v>82</v>
-      </c>
-      <c r="L98">
-        <v>0.25</v>
+      <c r="J98" s="7">
+        <f>J92+1</f>
+        <v>44308</v>
       </c>
     </row>
     <row r="99" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J99" s="9"/>
+      <c r="J99" s="7"/>
     </row>
     <row r="100" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J100" s="9"/>
-    </row>
-    <row r="102" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J102" s="6">
-        <f>J96+1</f>
-        <v>44308</v>
-      </c>
-      <c r="L102">
-        <f>SUM(L103:L105)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J103" s="6"/>
-      <c r="L103">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J104" s="6"/>
-      <c r="L104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J105" s="6"/>
+      <c r="J100" s="7"/>
+    </row>
+    <row r="101" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J101" s="7"/>
+    </row>
+    <row r="102" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I105" s="5"/>
+      <c r="J105" s="6">
+        <f>J98+1</f>
+        <v>44309</v>
+      </c>
       <c r="L105">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F106" s="5"/>
+        <f>SUM(L106:L109)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
       <c r="J106" s="6"/>
-    </row>
-    <row r="107" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F107" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="108" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F108" s="5">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G108" s="5">
-        <v>9.375E-2</v>
-      </c>
-    </row>
-    <row r="109" spans="6:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J109" s="6">
-        <f>J102+1</f>
-        <v>44309</v>
+      <c r="K106" t="s">
+        <v>72</v>
+      </c>
+      <c r="L106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="I107" s="5"/>
+      <c r="J107" s="6"/>
+      <c r="K107" t="s">
+        <v>73</v>
+      </c>
+      <c r="L107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="I108" s="5"/>
+      <c r="J108" s="6"/>
+      <c r="K108" t="s">
+        <v>74</v>
+      </c>
+      <c r="L108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="I109" s="5"/>
+      <c r="J109" s="6"/>
+      <c r="K109" t="s">
+        <v>75</v>
       </c>
       <c r="L109">
-        <f>SUM(L110:L116)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="H110" s="5"/>
-      <c r="J110" s="6"/>
-      <c r="K110" t="s">
-        <v>72</v>
-      </c>
-      <c r="L110">
-        <v>2</v>
-      </c>
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
     </row>
     <row r="111" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J111" s="6"/>
-      <c r="K111" t="s">
-        <v>73</v>
-      </c>
-      <c r="L111">
-        <v>2</v>
-      </c>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
     </row>
     <row r="112" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="J112" s="6"/>
-      <c r="K112" t="s">
-        <v>74</v>
-      </c>
-      <c r="L112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J113" s="6"/>
-      <c r="K113" t="s">
-        <v>75</v>
-      </c>
-      <c r="L113">
-        <v>4</v>
-      </c>
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
     </row>
     <row r="114" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J114" s="6"/>
+      <c r="J114" s="6">
+        <f>J105+1</f>
+        <v>44310</v>
+      </c>
+      <c r="L114">
+        <f>SUM(L115:L119)</f>
+        <v>3.25</v>
+      </c>
     </row>
     <row r="115" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J115" s="6"/>
+      <c r="K115" t="s">
+        <v>76</v>
+      </c>
+      <c r="L115">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="116" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J116" s="6"/>
+      <c r="K116" t="s">
+        <v>77</v>
+      </c>
+      <c r="L116">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="117" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J117" s="6"/>
+      <c r="K117" t="s">
+        <v>79</v>
+      </c>
+      <c r="L117">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="118" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J118" s="6">
-        <f>J109+1</f>
-        <v>44310</v>
+      <c r="J118" s="6"/>
+      <c r="K118" t="s">
+        <v>80</v>
       </c>
       <c r="L118">
-        <f>SUM(L119:L123)</f>
-        <v>3.25</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="119" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J119" s="6"/>
       <c r="K119" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="L119">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="120" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J120" s="6"/>
-      <c r="K120" t="s">
-        <v>77</v>
-      </c>
-      <c r="L120">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="121" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J121" s="6"/>
-      <c r="K121" t="s">
-        <v>79</v>
-      </c>
-      <c r="L121">
-        <v>0.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J122" s="6"/>
-      <c r="K122" t="s">
-        <v>80</v>
+      <c r="J122" s="6">
+        <f>J114+1</f>
+        <v>44311</v>
       </c>
       <c r="L122">
-        <v>0.25</v>
+        <f>SUM(L123:L128)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J123" s="6"/>
       <c r="K123" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L123">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J124" s="6">
-        <f>J118+1</f>
-        <v>44311</v>
+      <c r="J124" s="6"/>
+      <c r="K124" t="s">
+        <v>84</v>
       </c>
       <c r="L124">
-        <f>SUM(L125:L130)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J125" s="6"/>
       <c r="K125" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L125">
         <v>1</v>
@@ -1676,7 +1686,7 @@
     <row r="126" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J126" s="6"/>
       <c r="K126" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L126">
         <v>1</v>
@@ -1685,114 +1695,292 @@
     <row r="127" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J127" s="6"/>
       <c r="K127" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L127">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J128" s="6"/>
       <c r="K128" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="L128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K129" t="s">
-        <v>87</v>
-      </c>
-      <c r="L129">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="6:12" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K131" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L131" s="13">
+        <f>L132+L137+L143+L149+L156+L166+L173</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J132" s="7">
+        <v>44305</v>
+      </c>
+      <c r="L132">
+        <f>SUM(L133:L135)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J133" s="7"/>
+    </row>
+    <row r="134" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J134" s="7"/>
+    </row>
+    <row r="135" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J135" s="7"/>
+    </row>
+    <row r="136" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F136" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="137" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F137" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G137" s="5">
+        <v>9.375E-2</v>
+      </c>
+      <c r="J137" s="7">
+        <f>J132+1</f>
+        <v>44306</v>
+      </c>
+      <c r="L137">
+        <f>SUM(L138:L140)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J138" s="7"/>
+    </row>
+    <row r="139" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J139" s="7"/>
+    </row>
+    <row r="140" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J140" s="7"/>
+    </row>
+    <row r="143" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J143" s="9">
+        <f>J137+1</f>
+        <v>44307</v>
+      </c>
+      <c r="L143" s="12">
+        <f>SUM(L144:L147)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="J144" s="9"/>
+    </row>
+    <row r="145" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J145" s="9"/>
+    </row>
+    <row r="146" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J146" s="9"/>
+    </row>
+    <row r="147" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J147" s="9"/>
+    </row>
+    <row r="149" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J149" s="7">
+        <f>J143+1</f>
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="150" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J150" s="7"/>
+    </row>
+    <row r="151" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J151" s="7"/>
+    </row>
+    <row r="152" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J152" s="7"/>
+    </row>
+    <row r="156" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J156" s="6">
+        <f>J149+1</f>
+        <v>44309</v>
+      </c>
+      <c r="L156">
+        <f>SUM(L157:L160)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J157" s="6"/>
+    </row>
+    <row r="158" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J158" s="6"/>
+    </row>
+    <row r="159" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J159" s="6"/>
+    </row>
+    <row r="160" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J160" s="6"/>
+    </row>
+    <row r="161" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J161" s="5"/>
+    </row>
+    <row r="162" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J162" s="5"/>
+    </row>
+    <row r="163" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J163" s="5"/>
+    </row>
+    <row r="165" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J165" s="6">
+        <f>J156+1</f>
+        <v>44310</v>
+      </c>
+      <c r="L165">
+        <f>SUM(L166:L170)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J166" s="6"/>
+    </row>
+    <row r="167" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J167" s="6"/>
+    </row>
+    <row r="168" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J168" s="6"/>
+    </row>
+    <row r="169" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J169" s="6"/>
+    </row>
+    <row r="170" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J170" s="6"/>
+    </row>
+    <row r="173" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J173" s="6">
+        <f>J165+1</f>
+        <v>44311</v>
+      </c>
+      <c r="L173">
+        <f>SUM(L174:L179)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J174" s="6"/>
+    </row>
+    <row r="175" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J175" s="6"/>
+    </row>
+    <row r="176" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J176" s="6"/>
+    </row>
+    <row r="177" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J177" s="6"/>
+    </row>
+    <row r="178" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J178" s="6"/>
+    </row>
+    <row r="179" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J179" s="6"/>
+    </row>
+    <row r="182" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K182" t="s">
         <v>70</v>
       </c>
-      <c r="L135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K136" t="s">
+      <c r="L182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K183" t="s">
         <v>69</v>
       </c>
-      <c r="L136">
+      <c r="L183">
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L137" t="s">
+    <row r="184" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L184" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="138" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L138" t="s">
+    <row r="185" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L185" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L139" t="s">
+    <row r="186" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L186" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="140" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L140" t="s">
+    <row r="187" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L187" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="141" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L141" t="s">
+    <row r="188" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L188" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="142" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L142" t="s">
+    <row r="189" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L189" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="143" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="L143" s="4" t="s">
+    <row r="190" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L190" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="144" spans="11:12" x14ac:dyDescent="0.3">
-      <c r="K144" s="4"/>
-      <c r="L144" t="s">
+    <row r="191" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K191" s="4"/>
+      <c r="L191" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="156" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K156" t="s">
+    <row r="203" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K203" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="157" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K157" t="s">
+    <row r="204" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K204" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="160" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K160" t="s">
+    <row r="207" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K207" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="161" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K161" t="s">
+    <row r="208" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K208" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="J90:J94"/>
-    <mergeCell ref="J96:J100"/>
-    <mergeCell ref="J102:J106"/>
-    <mergeCell ref="J109:J116"/>
-    <mergeCell ref="J118:J122"/>
-    <mergeCell ref="J124:J128"/>
+  <mergeCells count="27">
+    <mergeCell ref="J173:J179"/>
+    <mergeCell ref="J137:J140"/>
+    <mergeCell ref="J143:J147"/>
+    <mergeCell ref="J149:J152"/>
+    <mergeCell ref="J156:J160"/>
+    <mergeCell ref="J165:J170"/>
+    <mergeCell ref="J122:J128"/>
+    <mergeCell ref="J81:J84"/>
+    <mergeCell ref="J86:J89"/>
+    <mergeCell ref="J105:J109"/>
+    <mergeCell ref="J98:J101"/>
+    <mergeCell ref="J132:J135"/>
+    <mergeCell ref="J92:J96"/>
+    <mergeCell ref="J114:J119"/>
     <mergeCell ref="J74:J77"/>
     <mergeCell ref="J3:J10"/>
     <mergeCell ref="J12:J16"/>
@@ -1806,7 +1994,6 @@
     <mergeCell ref="J53:J55"/>
     <mergeCell ref="J57:J58"/>
     <mergeCell ref="J60:J61"/>
-    <mergeCell ref="J81:J88"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
implemented new graph after Nadine's remarks
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785ACA16-9AE2-472C-B29A-60AEA1E790DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B4308-FF6B-43B6-B2E0-6D31AEBFE2D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="99">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -299,10 +299,37 @@
     <t>Correctif: recherche des bornes des différents ranges pour la vérification globale</t>
   </si>
   <si>
-    <t>modification des ranges nommées attachées au classeur entier</t>
-  </si>
-  <si>
     <t>Semaine du 26 Avril au 02 Mai 2021</t>
+  </si>
+  <si>
+    <t>Lors de la création d'une nouvelle facture from autre feuille que template, prendre cettte feuille comme base et vider la table d'appel de fond</t>
+  </si>
+  <si>
+    <t>Recréer le filigrane pour éviter le dérèglement des couleurs à l'impression</t>
+  </si>
+  <si>
+    <t>Refaire le graphique Total devis TTC selon modèle de Nadine</t>
+  </si>
+  <si>
+    <t>A discuter</t>
+  </si>
+  <si>
+    <t>Taxe d'ameublement trop petit pour être visible</t>
+  </si>
+  <si>
+    <t>Faire remarquer que le titre change si taxe d'ameublement ou pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Enregistrement des infos clients</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>08h30</t>
   </si>
 </sst>
 </file>
@@ -742,8 +769,8 @@
   </sheetPr>
   <dimension ref="C1:L208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D123" workbookViewId="0">
-      <selection activeCell="K139" sqref="K139"/>
+    <sheetView tabSelected="1" topLeftCell="F123" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1712,65 +1739,97 @@
     </row>
     <row r="131" spans="6:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="K131" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L131" s="13">
         <f>L132+L137+L143+L149+L156+L166+L173</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J132" s="7">
-        <v>44305</v>
+        <v>44312</v>
+      </c>
+      <c r="K132" t="s">
+        <v>89</v>
       </c>
       <c r="L132">
-        <f>SUM(L133:L135)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J133" s="7"/>
+      <c r="K133" t="s">
+        <v>90</v>
+      </c>
+      <c r="L133">
+        <v>1</v>
+      </c>
     </row>
     <row r="134" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J134" s="7"/>
+      <c r="K134" t="s">
+        <v>91</v>
+      </c>
+      <c r="L134">
+        <v>1</v>
+      </c>
     </row>
     <row r="135" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J135" s="7"/>
     </row>
     <row r="136" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F136" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="137" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F137" s="5">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G137" s="5">
-        <v>9.375E-2</v>
+      <c r="F137" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G137" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="J137" s="7">
         <f>J132+1</f>
-        <v>44306</v>
+        <v>44313</v>
+      </c>
+      <c r="K137" t="s">
+        <v>91</v>
       </c>
       <c r="L137">
-        <f>SUM(L138:L140)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J138" s="7"/>
+      <c r="L138" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="139" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J139" s="7"/>
     </row>
     <row r="140" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F140" t="s">
+        <v>92</v>
+      </c>
       <c r="J140" s="7"/>
+    </row>
+    <row r="141" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="G141" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="142" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="G142" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="143" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J143" s="9">
         <f>J137+1</f>
-        <v>44307</v>
+        <v>44314</v>
       </c>
       <c r="L143" s="12">
         <f>SUM(L144:L147)</f>
@@ -1792,7 +1851,7 @@
     <row r="149" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J149" s="7">
         <f>J143+1</f>
-        <v>44308</v>
+        <v>44315</v>
       </c>
     </row>
     <row r="150" spans="10:12" x14ac:dyDescent="0.3">
@@ -1807,7 +1866,7 @@
     <row r="156" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J156" s="6">
         <f>J149+1</f>
-        <v>44309</v>
+        <v>44316</v>
       </c>
       <c r="L156">
         <f>SUM(L157:L160)</f>
@@ -1838,7 +1897,7 @@
     <row r="165" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J165" s="6">
         <f>J156+1</f>
-        <v>44310</v>
+        <v>44317</v>
       </c>
       <c r="L165">
         <f>SUM(L166:L170)</f>
@@ -1863,7 +1922,7 @@
     <row r="173" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J173" s="6">
         <f>J165+1</f>
-        <v>44311</v>
+        <v>44318</v>
       </c>
       <c r="L173">
         <f>SUM(L174:L179)</f>

</xml_diff>

<commit_message>
implemented a generic function to save ranges + applied it to Appel de fond
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B4308-FF6B-43B6-B2E0-6D31AEBFE2D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AD6896-09D3-44EC-8665-21A93488E8FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -326,10 +326,25 @@
     <t>Enregistrement des infos clients</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>08h30</t>
+    <t>Enregistrement des détails de la facture</t>
+  </si>
+  <si>
+    <t>Enregistrement des devis et DMPs</t>
+  </si>
+  <si>
+    <t>Enregistrement de la typologie client</t>
+  </si>
+  <si>
+    <t>7h45</t>
+  </si>
+  <si>
+    <t>Insertion d'une nouvelle facture: mise à jour des ranges nommés</t>
+  </si>
+  <si>
+    <t>Export d'une nouvelle facture: mise à jour des ranges nommés</t>
+  </si>
+  <si>
+    <t>Export appel de fond avec ne fonction générique</t>
   </si>
 </sst>
 </file>
@@ -769,8 +784,8 @@
   </sheetPr>
   <dimension ref="C1:L208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F123" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="G168" workbookViewId="0">
+      <selection activeCell="K178" sqref="K178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1743,7 +1758,7 @@
       </c>
       <c r="L131" s="13">
         <f>L132+L137+L143+L149+L156+L166+L173</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="6:12" x14ac:dyDescent="0.3">
@@ -1780,15 +1795,15 @@
     </row>
     <row r="136" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F136" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="137" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F137" s="5" t="s">
-        <v>97</v>
+      <c r="F137" s="5">
+        <v>0.5</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J137" s="7">
         <f>J132+1</f>
@@ -1831,9 +1846,11 @@
         <f>J137+1</f>
         <v>44314</v>
       </c>
-      <c r="L143" s="12">
-        <f>SUM(L144:L147)</f>
-        <v>0</v>
+      <c r="K143" t="s">
+        <v>96</v>
+      </c>
+      <c r="L143">
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="6:12" x14ac:dyDescent="0.3">
@@ -1853,6 +1870,12 @@
         <f>J143+1</f>
         <v>44315</v>
       </c>
+      <c r="K149" t="s">
+        <v>97</v>
+      </c>
+      <c r="L149">
+        <v>2</v>
+      </c>
     </row>
     <row r="150" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J150" s="7"/>
@@ -1885,16 +1908,16 @@
     <row r="160" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J160" s="6"/>
     </row>
-    <row r="161" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J161" s="5"/>
     </row>
-    <row r="162" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J162" s="5"/>
     </row>
-    <row r="163" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J163" s="5"/>
     </row>
-    <row r="165" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J165" s="6">
         <f>J156+1</f>
         <v>44317</v>
@@ -1904,39 +1927,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J166" s="6"/>
     </row>
-    <row r="167" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J167" s="6"/>
     </row>
-    <row r="168" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J168" s="6"/>
     </row>
-    <row r="169" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J169" s="6"/>
     </row>
-    <row r="170" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J170" s="6"/>
     </row>
-    <row r="173" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J173" s="6">
         <f>J165+1</f>
         <v>44318</v>
       </c>
+      <c r="K173" t="s">
+        <v>98</v>
+      </c>
       <c r="L173">
-        <f>SUM(L174:L179)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="10:12" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F174" t="s">
+        <v>101</v>
+      </c>
       <c r="J174" s="6"/>
-    </row>
-    <row r="175" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K174" t="s">
+        <v>99</v>
+      </c>
+      <c r="L174">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="175" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F175" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G175" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="J175" s="6"/>
-    </row>
-    <row r="176" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K175" t="s">
+        <v>102</v>
+      </c>
+      <c r="L175">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="176" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J176" s="6"/>
+      <c r="K176" t="s">
+        <v>103</v>
+      </c>
+      <c r="L176">
+        <v>3</v>
+      </c>
     </row>
     <row r="177" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J177" s="6"/>
@@ -1964,62 +2016,76 @@
       </c>
     </row>
     <row r="184" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L184" t="s">
-        <v>71</v>
+      <c r="K184" t="s">
+        <v>102</v>
+      </c>
+      <c r="L184">
+        <v>0.5</v>
       </c>
     </row>
     <row r="185" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L185" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="186" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L186" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="187" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L187" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="188" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L188" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="189" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L189" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="190" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L190" s="4" t="s">
-        <v>67</v>
+      <c r="K185" t="s">
+        <v>103</v>
+      </c>
+      <c r="L185">
+        <v>3</v>
       </c>
     </row>
     <row r="191" spans="10:12" x14ac:dyDescent="0.3">
       <c r="K191" s="4"/>
-      <c r="L191" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="203" spans="11:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L197" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="198" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L198" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="199" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L199" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="200" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L200" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="201" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L201" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="202" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L202" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="203" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K203" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="204" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="L203" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="204" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K204" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="207" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="L204" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="207" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K207" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="208" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="11:12" x14ac:dyDescent="0.3">
       <c r="K208" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
implemented the export of the factures d'acompte using the generic function
</commit_message>
<xml_diff>
--- a/Carnet de bord Solomas Ebenisterie.xlsx
+++ b/Carnet de bord Solomas Ebenisterie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZA\Documents\Solomas Ebenisterie\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AD6896-09D3-44EC-8665-21A93488E8FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE53CEB-2D12-4142-80FE-F76CAB0D688E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{5420C4B1-4F87-4C7E-AB53-3A2EFC62172F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
   <si>
     <t>Mercredi 10/03</t>
   </si>
@@ -338,13 +338,19 @@
     <t>7h45</t>
   </si>
   <si>
-    <t>Insertion d'une nouvelle facture: mise à jour des ranges nommés</t>
-  </si>
-  <si>
     <t>Export d'une nouvelle facture: mise à jour des ranges nommés</t>
   </si>
   <si>
     <t>Export appel de fond avec ne fonction générique</t>
+  </si>
+  <si>
+    <t>Utilisation de la fonction générique pour exporter les factures d'acompte</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>13h45</t>
   </si>
 </sst>
 </file>
@@ -784,8 +790,8 @@
   </sheetPr>
   <dimension ref="C1:L208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G168" workbookViewId="0">
-      <selection activeCell="K178" sqref="K178"/>
+    <sheetView tabSelected="1" topLeftCell="E168" workbookViewId="0">
+      <selection activeCell="L178" sqref="L178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1956,7 +1962,7 @@
     </row>
     <row r="174" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F174" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J174" s="6"/>
       <c r="K174" t="s">
@@ -1967,15 +1973,15 @@
       </c>
     </row>
     <row r="175" spans="6:12" x14ac:dyDescent="0.3">
-      <c r="F175" s="5">
-        <v>0.5</v>
+      <c r="F175" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="G175" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="J175" s="6"/>
       <c r="K175" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L175">
         <v>0.5</v>
@@ -1984,7 +1990,7 @@
     <row r="176" spans="6:12" x14ac:dyDescent="0.3">
       <c r="J176" s="6"/>
       <c r="K176" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L176">
         <v>3</v>
@@ -1992,6 +1998,12 @@
     </row>
     <row r="177" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J177" s="6"/>
+      <c r="K177" t="s">
+        <v>103</v>
+      </c>
+      <c r="L177">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="178" spans="10:12" x14ac:dyDescent="0.3">
       <c r="J178" s="6"/>
@@ -2017,7 +2029,7 @@
     </row>
     <row r="184" spans="10:12" x14ac:dyDescent="0.3">
       <c r="K184" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L184">
         <v>0.5</v>
@@ -2025,7 +2037,7 @@
     </row>
     <row r="185" spans="10:12" x14ac:dyDescent="0.3">
       <c r="K185" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L185">
         <v>3</v>

</xml_diff>